<commit_message>
Update figures with correct mean accu rate
</commit_message>
<xml_diff>
--- a/figure06_maps_10Be_model_data_antarctica/mean_10Be_data_holocene.xlsx
+++ b/figure06_maps_10Be_model_data_antarctica/mean_10Be_data_holocene.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acauquoin/Documents/Mes_manuscrits/10Be_Holocene_Antarctica/figures/figure06_maps_10Be_model_data_antarctica/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210692A8-2735-DF46-9BB0-DD4C097F4E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3532C666-7378-514D-A46D-14640350C1FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9840" yWindow="12820" windowWidth="27240" windowHeight="16440" xr2:uid="{74A6B4C7-0AD0-6B43-B0B4-B6C90525EC13}"/>
+    <workbookView xWindow="21320" yWindow="5580" windowWidth="27240" windowHeight="16440" xr2:uid="{74A6B4C7-0AD0-6B43-B0B4-B6C90525EC13}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="mean_10Be_data_holocene" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -47,24 +47,9 @@
     <t>Longitude</t>
   </si>
   <si>
-    <t xml:space="preserve"> concobs </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> accuobs </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> fluxobs </t>
-  </si>
-  <si>
     <t>Siple Dome</t>
   </si>
   <si>
-    <t>WD</t>
-  </si>
-  <si>
-    <t>South Pole</t>
-  </si>
-  <si>
     <t>EDML</t>
   </si>
   <si>
@@ -87,6 +72,21 @@
   </si>
   <si>
     <t>SPICE</t>
+  </si>
+  <si>
+    <t>PS1</t>
+  </si>
+  <si>
+    <t>Wais Divide</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fluxobs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> accuobs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> concobs</t>
   </si>
 </sst>
 </file>
@@ -94,7 +94,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -145,10 +145,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -494,7 +494,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -516,18 +516,18 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" s="5">
         <v>-81.654302999999999</v>
@@ -539,15 +539,15 @@
         <v>0.23799999999999999</v>
       </c>
       <c r="E2" s="5">
-        <v>15.5</v>
+        <v>14.2</v>
       </c>
       <c r="F2" s="5">
-        <v>116.42484</v>
+        <v>107.16641298833079</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B3" s="5">
         <v>-79.783332999999999</v>
@@ -559,15 +559,15 @@
         <v>0.14299999999999999</v>
       </c>
       <c r="E3" s="5">
-        <v>21.9</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="F3" s="5">
-        <v>98.836451999999994</v>
+        <v>91.143455098934552</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B4" s="5">
         <v>-90</v>
@@ -579,15 +579,15 @@
         <v>0.39</v>
       </c>
       <c r="E4" s="5">
-        <v>9.51</v>
+        <v>8.7200000000000006</v>
       </c>
       <c r="F4" s="5">
-        <v>117.05288400000001</v>
+        <v>107.83866057838662</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B5" s="5">
         <v>-75</v>
@@ -599,35 +599,35 @@
         <v>0.39900000000000002</v>
       </c>
       <c r="E5" s="5">
-        <v>6.98</v>
+        <v>6.28</v>
       </c>
       <c r="F5" s="5">
-        <v>87.895231199999998</v>
+        <v>79.455859969558603</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B6" s="5">
-        <v>-74.650000000000006</v>
+        <v>-75.06</v>
       </c>
       <c r="C6" s="5">
-        <v>124.166667</v>
+        <v>123.21</v>
       </c>
       <c r="D6" s="3">
         <v>0.67700000000000005</v>
       </c>
       <c r="E6" s="5">
-        <v>2.72</v>
+        <v>2.5</v>
       </c>
       <c r="F6" s="5">
-        <v>58.115846400000002</v>
+        <v>53.67</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B7" s="5">
         <v>-75.099999999999994</v>
@@ -636,38 +636,38 @@
         <v>123.35</v>
       </c>
       <c r="D7" s="3">
-        <v>0.56000000000000005</v>
+        <v>0.59</v>
       </c>
       <c r="E7" s="5">
-        <v>2.5299999999999998</v>
+        <v>2.31</v>
       </c>
       <c r="F7" s="5">
-        <v>44.714207999999999</v>
+        <v>43.217275494672755</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B8" s="6">
-        <v>-74.650000000000006</v>
+        <v>-74.39</v>
       </c>
       <c r="C8" s="6">
-        <v>124.17</v>
+        <v>124.1</v>
       </c>
       <c r="D8" s="4">
         <v>0.51</v>
       </c>
       <c r="E8" s="6">
-        <v>3.22</v>
+        <v>2.99</v>
       </c>
       <c r="F8" s="6">
-        <v>51.827832000000001</v>
+        <v>48.354261796042621</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B9" s="5">
         <v>-78.466667000000001</v>
@@ -679,15 +679,15 @@
         <v>0.88100000000000001</v>
       </c>
       <c r="E9" s="5">
-        <v>2.1</v>
+        <v>1.93</v>
       </c>
       <c r="F9" s="5">
-        <v>58.389156</v>
+        <v>53.917110603754438</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B10" s="5">
         <v>-77.316666999999995</v>
@@ -699,15 +699,15 @@
         <v>0.87</v>
       </c>
       <c r="E10" s="5">
-        <v>3.5</v>
+        <v>3.21</v>
       </c>
       <c r="F10" s="5">
-        <v>96.100200000000001</v>
+        <v>88.555936073059357</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B11" s="5">
         <v>-80.366667000000007</v>
@@ -719,15 +719,15 @@
         <v>1.012</v>
       </c>
       <c r="E11" s="5">
-        <v>2.5</v>
+        <v>2.29</v>
       </c>
       <c r="F11" s="5">
-        <v>79.846800000000002</v>
+        <v>73.486808726534761</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B12" s="5">
         <v>-89.98</v>
@@ -739,10 +739,10 @@
         <v>0.34899999999999998</v>
       </c>
       <c r="E12" s="5">
-        <v>8.9</v>
+        <v>8.16</v>
       </c>
       <c r="F12" s="5">
-        <v>98.028515999999996</v>
+        <v>90.304414003044144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>